<commit_message>
Read Excel Code Push
</commit_message>
<xml_diff>
--- a/TestData/login_data.xlsx
+++ b/TestData/login_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pratham.kumar\PycharmProjects\LearnSelenium\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72938682-7BED-4DF1-B1F4-700450E7EEA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473ACAEF-19FC-4F79-BAC5-9EDEF51F5970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4596" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,19 +28,19 @@
     <t>password</t>
   </si>
   <si>
+    <t>expected</t>
+  </si>
+  <si>
     <t>new_user@example.com</t>
   </si>
   <si>
     <t>testuser@456</t>
   </si>
   <si>
+    <t>fail</t>
+  </si>
+  <si>
     <t>qa@impactanalytics.co</t>
-  </si>
-  <si>
-    <t>expected</t>
-  </si>
-  <si>
-    <t>fail</t>
   </si>
   <si>
     <t>pass</t>
@@ -427,7 +427,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,26 +444,26 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
@@ -471,21 +471,21 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>

</xml_diff>